<commit_message>
updated model eval and training dict
</commit_message>
<xml_diff>
--- a/data/meta/training_dict_bra.xlsx
+++ b/data/meta/training_dict_bra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ucn\Education\20202\DSSGx\data\meta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{038D21F9-9291-4DA5-8BC3-EC81D892C3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{890244A1-DCC8-4E2C-9010-676F5B048C2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +752,7 @@
         <v>49</v>
       </c>
       <c r="G12" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -798,7 +798,7 @@
         <v>49</v>
       </c>
       <c r="G14" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -867,7 +867,7 @@
         <v>49</v>
       </c>
       <c r="G17" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -890,7 +890,7 @@
         <v>49</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -913,7 +913,7 @@
         <v>49</v>
       </c>
       <c r="G19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
         <v>49</v>
       </c>
       <c r="G22" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1028,7 +1028,7 @@
         <v>49</v>
       </c>
       <c r="G24" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1051,7 +1051,7 @@
         <v>49</v>
       </c>
       <c r="G25" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1065,7 +1065,7 @@
         <v>38</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="E26" t="s">
         <v>39</v>
@@ -1074,7 +1074,7 @@
         <v>49</v>
       </c>
       <c r="G26" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1097,7 +1097,7 @@
         <v>49</v>
       </c>
       <c r="G27" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1143,7 +1143,7 @@
         <v>49</v>
       </c>
       <c r="G29" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>